<commit_message>
add featuring to reports
</commit_message>
<xml_diff>
--- a/providers/datos-proveedores.xlsx
+++ b/providers/datos-proveedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres.lopez.JDELECTRICOS\Documents\codes\send-mails-certificados-retenciones\providers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BB58A3-6B2A-454A-B740-E850A440D6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E99ABCD-CD37-4D8F-BE00-49D24E74AAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>correo</t>
   </si>
@@ -45,13 +45,13 @@
     <t>proveedor</t>
   </si>
   <si>
-    <t>abicdev26@gmail.com</t>
-  </si>
-  <si>
     <t>PROVEEDOR SIN CORREO</t>
   </si>
   <si>
     <t>PROVEEDOR SIN DOCUMENTO</t>
+  </si>
+  <si>
+    <t>japsequiposelectricos@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -422,7 +422,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -430,29 +430,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="G7" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -462,7 +457,13 @@
       <c r="G14" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{82EB093A-6084-421F-9BBF-BA2DE119727A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{DA64938E-3AEA-42DE-A9CF-E8E86374A4DF}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{748F209E-857A-4795-8C1E-F48A28D6F732}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{09CE7F0F-B878-49D4-9475-B96702AA9F11}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add .bat to production
</commit_message>
<xml_diff>
--- a/providers/datos-proveedores.xlsx
+++ b/providers/datos-proveedores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres.lopez.JDELECTRICOS\Documents\codes\send-mails-certificados-retenciones\providers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E99ABCD-CD37-4D8F-BE00-49D24E74AAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E994A544-EFD6-469D-8714-1BEC9FA055CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23985" yWindow="1590" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>correo</t>
   </si>
   <si>
-    <t>ACCESORIOS Y HERRAJES JM SAS</t>
-  </si>
-  <si>
     <t>ACDC ELECTRIC SAS</t>
-  </si>
-  <si>
-    <t>AGENCIA DE ADUANAS SERVICIOS</t>
   </si>
   <si>
     <t>proveedor</t>
@@ -392,7 +386,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +397,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -414,36 +408,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -458,12 +436,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{82EB093A-6084-421F-9BBF-BA2DE119727A}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{DA64938E-3AEA-42DE-A9CF-E8E86374A4DF}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{748F209E-857A-4795-8C1E-F48A28D6F732}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{09CE7F0F-B878-49D4-9475-B96702AA9F11}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DA64938E-3AEA-42DE-A9CF-E8E86374A4DF}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{09CE7F0F-B878-49D4-9475-B96702AA9F11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add timer to run send mails
</commit_message>
<xml_diff>
--- a/providers/datos-proveedores.xlsx
+++ b/providers/datos-proveedores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres.lopez.JDELECTRICOS\Documents\codes\send-mails-certificados-retenciones\providers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E994A544-EFD6-469D-8714-1BEC9FA055CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00A2A24-56F8-4944-B514-0ED25747B614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23985" yWindow="1590" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18225" yWindow="6150" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,21 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>correo</t>
-  </si>
-  <si>
-    <t>ACDC ELECTRIC SAS</t>
   </si>
   <si>
     <t>proveedor</t>
   </si>
   <si>
-    <t>PROVEEDOR SIN CORREO</t>
+    <t>ACCESORIOS Y HERRAJES JM SAS</t>
   </si>
   <si>
-    <t>PROVEEDOR SIN DOCUMENTO</t>
+    <t>ACDC ELECTRIC SAS</t>
   </si>
   <si>
     <t>japsequiposelectricos@gmail.com</t>
@@ -52,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +73,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE3E3E3"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -98,10 +100,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -386,18 +390,19 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -405,24 +410,23 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -435,11 +439,7 @@
       <c r="G14" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DA64938E-3AEA-42DE-A9CF-E8E86374A4DF}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{09CE7F0F-B878-49D4-9475-B96702AA9F11}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>